<commit_message>
update to cross mapping file
</commit_message>
<xml_diff>
--- a/docs/rare diseases/GEL_openEHR_Cross_references.xlsx
+++ b/docs/rare diseases/GEL_openEHR_Cross_references.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="24" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="1137">
   <si>
     <t>Full Name of Responsible Consultant (12774.4)</t>
   </si>
@@ -4541,6 +4541,1415 @@
 contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
 contains CLUSTER b_a[openEHR-EHR-CLUSTER.analytical_technique_gel.v0]
 where a/name/value='GEL Rare disease investigations laboratory tests'</t>
+  </si>
+  <si>
+    <t>not modelled separately - part of each individual non-imaging section</t>
+  </si>
+  <si>
+    <t>This data item is used in each of the non-imaging diagnostics sections and has been modelled differently in each. See details in each section.</t>
+  </si>
+  <si>
+    <t>29524.1</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0002]/events[at0003]/data[at0001]/items[at1023]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.pulse.v1])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Patient_status
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.patient_status_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>this data item is also used in the other non-imaging sections, and the b_a/name/value pair should be replaced with the appropriate section heading, e.g. Forced vital capacity, ECG diagnostics, Sleep test etc. Note that the section headings are case sensitive.</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0002, 'Filename of uploaded copy of report']/value/value as Filename_of_uploaded_copy_of_report
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.multimedia.v1])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001, 'Analysis type']/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.analytical_technique_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0002]/events[at0003]/data[at0001]/items[at0004]/value/magnitude as Heart_Rate
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.pulse.v1])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0002]/events[at0003]/data[at0001]/items[at0005]/value/value as Regular,
+    b_b/data[at0002]/events[at0003]/data[at0001]/items[at1055]/value/value as Irregular_type
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.pulse.v1])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>this data item is filled from two separate data points in the archetype, and hence the AQL query brings back both. Some business logic will be needed to combine the two values.</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0002]/events[at0003]/data[at0001]/items[at1022]/value/value as Heart_observations
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.pulse.v1])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Heart observations'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0127]/items[at0052]/items[at0044, 'FVC/expected FVC result']/value as FVC_expected_FVC_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.pulmonary_function.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Forced vital capacity'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001, 'Analysis type']/value/value as non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.analytical_technique_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Forced vital capacity'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0130]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.pulmonary_function.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Forced vital capacity'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0002]/value/value as Type_1_ECG
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0006]/value/value as High_RV_leads
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0010]/value/value as High_RV_in_which_lead
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0005]/items[at0006]/items[at0007]/value/magnitude as QT_interval
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ecg.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0005]/items[at0006]/items[at0012]/value/magnitude as PR_interval
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0005]/items[at0006]/items[at0014]/value/magnitude as QRS_duration
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0005]/items[at0006]/items[at0023]/items[at0021]/value/magnitude as QRS_axis
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0019]/value/value as Pre_excitation
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0011]/value/value as Abnormal_Q_waves
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0015]/value/value as Interventricular_delay
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ecg_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='ECG diagnostics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0004]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/value as Mean_sleep_latency_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0006]/value/magnitude as Number_of_SOREM
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0007]/value/magnitude as Total_sleep_time
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0008]/value/value as Sleep_related_breathing_parameters
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0009]/value/value as Sleep_efficiency
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/value as Periodic_limb_movements_in_sleep
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0013]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.sleep_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Sleep test'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Patient_status
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.patient_status_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0002]/value/value as Sodium_channel_blocker
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0005]/value/value as Sodium_channel_blocker_dosage
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0006]/value/magnitude as Body_weight_at_challenge
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0007]/value/magnitude as Calculated_drug_amount
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0008]/value/value as Dose_at_Type_1_ECG
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0009]/value/value as Total_amount_of_drug_given
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0016]/value/value as Reason_for_premature_termination
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_drug_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0015]/value/value as Premature_termination
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_drug_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0010]/value/value as High_RV_leads_used
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0014]/value/value as Lead_of_first_observation
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sodium_channel_blocker_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_drug_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0002]/value/value as Epinephrine_protocol
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0015]/value/value as Premature_termination
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_drug_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'
+</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0011]/value/value as Diagnostic_QT_prolongation
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0015]/value/value as Diagnostic_polymorphic_VT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0019]/value/value as Diagnostic_bidirectional_VT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0023]/value/value as Diagnostic_VPB_burden
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0027]/value/value as Diagnostic_VPB_frequency
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.epinephrine_challenge_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Cardiac drug challenge'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0004]/items[at0005]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.holter_monitor.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Holter monitor test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0009]/value/magnitude as VPB_burden_per_24_hours_magnitude
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.holter_monitor.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Holter monitor test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/value as Dynamic_type_1_ECG_pattern
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.holter_monitor.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Holter monitor test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0014]/value/value as QT_abnormalities_detected
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.holter_monitor.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Holter monitor test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0018]/value/value as QT_abnormality_description
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.holter_monitor.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Holter monitor test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0019]/value/value as Holter_monitor_abnormalities
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.holter_monitor.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Holter monitor test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0004]/items[at0005]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.signal_averaged_ecg.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Signal averaged ECG'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0009]/value/magnitude as FQRSd
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.signal_averaged_ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Signal averaged ECG'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/magnitude as HFLA
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.signal_averaged_ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Signal averaged ECG'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/magnitude as RMS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.signal_averaged_ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Signal averaged ECG'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0012]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.signal_averaged_ecg.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Signal averaged ECG'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0004]/items[at0005]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/value as Diagnostic_polymorphic_VT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0014]/value/value as Diagnostic_bidirectional_VT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0018]/value/value as Dynamic_type1_ECG_pattern
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0022]/value/value as Recovery_QTc_greater_than_480ms
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0026]/value/value as Exercise_test_additional_finding
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0027]/value/value as Vasoactive_medication
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0028]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.cardiac_exercise_test.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Exercise test cardiac'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0004]/items[at0005]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.electrophysiological_study_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Electrophysiological study'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0009]/value/magnitude as VERP
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.electrophysiological_study_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Electrophysiological study'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/value as Inducibility
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.electrophysiological_study_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Electrophysiological study'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0014]/value/value as Inducibility_intervals
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.electrophysiological_study_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Electrophysiological study'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0015]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.electrophysiological_study_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Electrophysiological study'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0006]/items[at0007]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Auditory brainstem response'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/value as Auditory_brainstem_response_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Auditory brainstem response'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Auditory brainstem response'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0006]/items[at0007]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Otoacustic emissions'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/value as Otoacustic_emissions_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Otoacustic emissions'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Otoacustic emissions'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0020]/items[at0021]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Right eye']/items[at0006]/value/magnitude as Axial_length_OD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Left eye']/items[at0006]/value/magnitude as Axial_length_OS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Right eye']/items[at0007]/value/magnitude as Central_corneal_thickness_OD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Left eye']/items[at0007]/value/magnitude as Central_corneal_thickness_OS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Right eye']/items[at0008]/value/magnitude as Corneal_diameter_OD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Left eye']/items[at0008]/value/magnitude as Corneal_diameter_OS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Right eye']/items[at0009]/value/magnitude as Keratometry_OD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0025, 'Left eye']/items[at0009]/value/magnitude as Keratometry_OS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0015]/value/value as Gonioscopy_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0026]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.ocular_malformation_metrics_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular malformation metrics'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0006]/items[at0007]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Visual field'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/magnitude as Central_visual_field_III_HVF_result_magnitude
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Visual field'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/magnitude as Continuous_central_visual_field_III_4_e_GVF_result_magnitude
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Visual field'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Visual field'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0068]/items[at0046]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.intraocular_pressure.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Ocular pressure'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002, 'Highest recorded left']/data[at0003]/items[at0061, 'Assessment']/value/value as Assessment_highest_left,
+    b_b/data[at0001]/events[at0002, 'Current right']/data[at0003]/items[at0061, 'Assessment']/value/value as Assessment_current_right,
+    b_b/data[at0001]/events[at0002, 'Current left']/data[at0003]/items[at0061, 'Assessment']/value/value as Assessment_current_left,
+    b_b/data[at0001]/events[at0002, 'Highest recorded right']/data[at0003]/items[at0061, 'Assessment']/value/value as Assessment_highest_right
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.intraocular_pressure.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular pressure'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002, 'Current right']/data[at0003]/items[at0042]/value/magnitude as Intraocular_pressure_OD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.intraocular_pressure.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular pressure'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002, 'Highest recorded right']/data[at0003]/items[at0042]/value/magnitude as Intraocular_pressure_highest_OD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.intraocular_pressure.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular pressure'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002, 'Current left']/data[at0003]/items[at0042]/value/magnitude as Intraocular_pressure_OS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.intraocular_pressure.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular pressure'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002, 'Highest recorded left']/data[at0003]/items[at0042]/value/magnitude as Intraocular_pressure_highest_OS
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.intraocular_pressure.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Ocular pressure'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0006]/items[at0007]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Colour plate test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/value as Ishihara_colour_plate_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Colour plate test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Colour plate test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0006]/items[at0007]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Electro-oculogram'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005, 'Arden ratio result']/value as Arden_ratio_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Electro-oculogram'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Electro-oculogram'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0006]/items[at0007]/value/value as Non_imaging_analytical_technique
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where a/name/value='GEL Rare disease investigations non imaging diagnostics'
+and b_a/name/value='Dark adaptation test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005, 'Dark adaptation final threshold result']/value/value as Dark_adaptation_final_threshold_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Dark adaptation test'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Assessment
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.non_imaging_diagnostic_test_gel.v0])
+where
+    a/name/value='GEL Rare disease investigations non imaging diagnostics' and
+    b_a/name/value='Dark adaptation test'</t>
+  </si>
+  <si>
+    <t>RD complete except Investigations</t>
+  </si>
+  <si>
+    <t>Investigations complete to row 266</t>
   </si>
 </sst>
 </file>
@@ -4615,7 +6024,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4641,8 +6050,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4677,8 +6088,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4691,6 +6105,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4703,6 +6118,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4980,8 +6396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5010,41 +6426,63 @@
       <c r="B2" s="11">
         <v>42914</v>
       </c>
+      <c r="C2" s="9" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="11"/>
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>42978</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1136</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
       <c r="B4" s="11"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
       <c r="B6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
       <c r="B7" s="11"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
       <c r="B8" s="11"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
       <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
       <c r="B11" s="11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
       <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
       <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
       <c r="B14" s="11"/>
     </row>
   </sheetData>
@@ -8887,10 +10325,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D327"/>
+  <dimension ref="A1:D345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="115" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView topLeftCell="A265" zoomScale="115" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="C267" sqref="C267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10355,7 +11793,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>29877.200000000001</v>
       </c>
@@ -10366,7 +11804,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>29875.1</v>
       </c>
@@ -10377,7 +11815,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>30107.200000000001</v>
       </c>
@@ -10388,39 +11826,57 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>30459.1</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C132" s="2" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>29524.1</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D133" s="2" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>34004.1</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C134" s="2" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>29501.200000000001</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C135" s="2" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>34838.1</v>
       </c>
@@ -10431,15 +11887,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>30178.2</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C137" s="2" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>30179.200000000001</v>
       </c>
@@ -10447,1594 +11906,2068 @@
         <v>255</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>34771.1</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C139" s="2" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>28040.1</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C140" s="2" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>28043.1</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C141" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
+        <v>29524.1</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
         <v>30180.2</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="3">
+    <row r="144" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
         <v>34774.1</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A144" s="3">
+      <c r="C144" s="2" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
         <v>30181.1</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" s="3">
-        <v>30183.200000000001</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>262</v>
-      </c>
       <c r="C145" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
-        <v>34777.1</v>
+        <v>29524.1</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>263</v>
+        <v>160</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>1034</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
+        <v>30183.200000000001</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>34777.1</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
         <v>31392.1</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" s="3">
+      <c r="C149" s="2" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
         <v>31394.1</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A149" s="3">
+      <c r="C150" s="2" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
         <v>31397.1</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B151" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" s="3">
+      <c r="C151" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
         <v>28600.1</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" s="3">
+      <c r="C152" s="2" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
         <v>28601.1</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" s="3">
+      <c r="C153" s="2" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
         <v>28602.1</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B154" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" s="3">
+      <c r="C154" s="2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
         <v>28605.1</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="3">
+      <c r="C155" s="2" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
         <v>28617.200000000001</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" s="3">
+      <c r="C156" s="2" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
         <v>28618.2</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" s="3">
+      <c r="C157" s="2" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
         <v>31396.1</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A157" s="3">
-        <v>30184.2</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A158" s="3">
-        <v>34780.1</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>275</v>
+      <c r="C158" s="2" t="s">
+        <v>1045</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
+        <v>30184.2</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>34780.1</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
         <v>30185.1</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B161" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A160" s="3">
+      <c r="C161" s="2" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
         <v>30186.1</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="3">
+      <c r="C162" s="2" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
         <v>30187.1</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" s="3">
+      <c r="C163" s="2" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
         <v>30190.1</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B164" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" s="3">
+      <c r="C164" s="2" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
         <v>30188.1</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B165" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="3">
+      <c r="C165" s="2" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
         <v>30189.1</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="3">
-        <v>31402.2</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="3">
-        <v>31400.2</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C166" s="2" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
-        <v>31403.200000000001</v>
+        <v>29524.1</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>284</v>
+        <v>160</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>38</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
-        <v>34786.1</v>
+        <v>31402.2</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="128" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
-        <v>31407.1</v>
+        <v>31400.2</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
+        <v>31403.200000000001</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A171" s="3">
+        <v>34786.1</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A172" s="3">
+        <v>31407.1</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A173" s="3">
         <v>31409.1</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B173" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" s="3">
+      <c r="C173" s="2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A174" s="3">
         <v>31410.1</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B174" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" s="3">
+      <c r="C174" s="2" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A175" s="3">
         <v>31474.1</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B175" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A173" s="3">
+      <c r="C175" s="2" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A176" s="3">
         <v>31412.1</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B176" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" s="3">
+      <c r="C176" s="2" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A177" s="3">
         <v>31413.1</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="3">
+      <c r="C177" s="2" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A178" s="3">
         <v>31421.1</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B178" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="3">
+      <c r="C178" s="2" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A179" s="3">
         <v>31415.1</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B179" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="3">
+      <c r="C179" s="2" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A180" s="3">
         <v>31416.1</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B180" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" s="3">
+      <c r="C180" s="2" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A181" s="3">
         <v>31417.1</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B181" s="2" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" s="3">
-        <v>31404.2</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="3">
-        <v>34789.1</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="3">
-        <v>31420.1</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="3">
-        <v>31421.1</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>292</v>
+      <c r="C181" s="2" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A182" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B182" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>1066</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
+        <v>31404.2</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A184" s="3">
+        <v>34789.1</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A185" s="3">
+        <v>31420.1</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A186" s="3">
+        <v>31421.1</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A187" s="3">
         <v>31415.1</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B187" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="3">
+      <c r="C187" s="2" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A188" s="3">
         <v>31422.1</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B188" s="2" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="3">
+      <c r="C188" s="2" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A189" s="3">
         <v>31423.1</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B189" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186" s="3">
+      <c r="C189" s="2" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A190" s="3">
         <v>31446.1</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B190" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187" s="3">
+      <c r="C190" s="2" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A191" s="3">
         <v>31424.1</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B191" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188" s="3">
+      <c r="C191" s="2" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A192" s="3">
         <v>31425.1</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B192" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="3">
-        <v>31432.2</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190" s="3">
-        <v>34792.1</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191" s="3">
-        <v>31433.1</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192" s="3">
-        <v>31434.1</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" s="3">
-        <v>31435.1</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>308</v>
+      <c r="C192" s="2" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A193" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B193" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>1066</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
+        <v>31432.2</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A195" s="3">
+        <v>34792.1</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A196" s="3">
+        <v>31433.1</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A197" s="3">
+        <v>31434.1</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A198" s="3">
+        <v>31435.1</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A199" s="3">
         <v>31436.1</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B199" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="3">
+      <c r="C199" s="2" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A200" s="3">
         <v>31462.1</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B200" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" s="3">
-        <v>31437.200000000001</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="3">
-        <v>34795.1</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="3">
-        <v>31442.1</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="3">
-        <v>31443.1</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="3">
-        <v>31444.1</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>315</v>
+      <c r="C200" s="2" t="s">
+        <v>1080</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
-        <v>31445.200000000001</v>
+        <v>31437.200000000001</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
-        <v>34798.1</v>
+        <v>34795.1</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
-        <v>31423.1</v>
+        <v>31442.1</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
-        <v>31446.1</v>
+        <v>31443.1</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
-        <v>31434.1</v>
+        <v>31444.1</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206" s="3">
-        <v>31447.1</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A206" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B206" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>1085</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
+        <v>31445.200000000001</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A208" s="3">
+        <v>34798.1</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A209" s="3">
+        <v>31423.1</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A210" s="3">
+        <v>31446.1</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A211" s="3">
+        <v>31434.1</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A212" s="3">
+        <v>31447.1</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A213" s="3">
         <v>31448.1</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B213" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" s="3">
+      <c r="C213" s="2" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A214" s="3">
         <v>31463.1</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B214" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A209" s="3">
-        <v>31449.200000000001</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A210" s="3">
-        <v>34801.1</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A211" s="3">
-        <v>31451.1</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A212" s="3">
-        <v>31452.1</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A213" s="3">
-        <v>31453.1</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A214" s="3">
-        <v>32992.1</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="C214" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A215" s="3">
-        <v>34804.1</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>327</v>
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A215" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B215" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>1093</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
-        <v>32999.1</v>
+        <v>31449.200000000001</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
-        <v>32993.1</v>
+        <v>34801.1</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
-        <v>34807.1</v>
+        <v>31451.1</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
-        <v>32998.1</v>
+        <v>31452.1</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
-        <v>30110.2</v>
+        <v>31453.1</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A221" s="3">
-        <v>30260.2</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>333</v>
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A221" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B221" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>38</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
-        <v>34813.1</v>
+        <v>32992.1</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
-        <v>28716.1</v>
+        <v>34804.1</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+        <v>327</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
-        <v>28717.1</v>
+        <v>32999.1</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A225" s="3">
-        <v>28731.1</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>337</v>
+        <v>328</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A225" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B225" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>1101</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="3">
-        <v>28732.1</v>
+        <v>32993.1</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
-        <v>28723.1</v>
+        <v>34807.1</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A228" s="3">
-        <v>28724.1</v>
+        <v>32998.1</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A229" s="3">
-        <v>28721.1</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>341</v>
+        <v>331</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A229" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B229" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>1104</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="3">
-        <v>28722.1</v>
+        <v>30110.2</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>342</v>
+        <v>332</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
+        <v>30260.2</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A232" s="3">
+        <v>34813.1</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A233" s="3">
+        <v>28716.1</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A234" s="3">
+        <v>28717.1</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A235" s="3">
+        <v>28731.1</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A236" s="3">
+        <v>28732.1</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A237" s="3">
+        <v>28723.1</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A238" s="3">
+        <v>28724.1</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A239" s="3">
+        <v>28721.1</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="192" x14ac:dyDescent="0.2">
+      <c r="A240" s="3">
+        <v>28722.1</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A241" s="3">
         <v>33077.1</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B241" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A232" s="3">
-        <v>30264.2</v>
-      </c>
-      <c r="B232" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A233" s="3">
-        <v>34816.1</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A234" s="3">
-        <v>30262.1</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A235" s="3">
-        <v>30263.1</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A236" s="3">
-        <v>30265.200000000001</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A237" s="3">
-        <v>34819.1</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A238" s="3">
-        <v>28713.1</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A239" s="3">
-        <v>28714.1</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A240" s="3">
-        <v>30266.1</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A241" s="3">
-        <v>30267.1</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A242" s="3">
-        <v>30269.200000000001</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>354</v>
+      <c r="C241" s="2" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A242" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B242" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>38</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
-        <v>34822.1</v>
+        <v>30264.2</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A244" s="3">
-        <v>30268.1</v>
+        <v>34816.1</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
-        <v>30271.200000000001</v>
+        <v>30262.1</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A246" s="3">
-        <v>34825.1</v>
+        <v>30263.1</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A247" s="3">
-        <v>30270.1</v>
-      </c>
-      <c r="B247" s="2" t="s">
-        <v>359</v>
+        <v>347</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A247" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B247" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>1119</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="3">
-        <v>30276.2</v>
+        <v>30265.200000000001</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
-        <v>34828.1</v>
+        <v>34819.1</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
-        <v>30275.200000000001</v>
+        <v>28713.1</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
-        <v>30291.200000000001</v>
+        <v>28714.1</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A252" s="3">
-        <v>34831.1</v>
+        <v>30266.1</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
-        <v>30281.1</v>
+        <v>30267.1</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A254" s="3">
-        <v>30282.1</v>
-      </c>
-      <c r="B254" s="2" t="s">
-        <v>366</v>
+        <v>353</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="288" x14ac:dyDescent="0.2">
+      <c r="A254" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B254" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
-        <v>30279.1</v>
+        <v>30269.200000000001</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A256" s="3">
-        <v>30280.1</v>
+        <v>34822.1</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
-        <v>30286.1</v>
+        <v>30268.1</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258" s="3">
-        <v>30287.1</v>
-      </c>
-      <c r="B258" s="2" t="s">
-        <v>370</v>
+        <v>356</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A258" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B258" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
-        <v>30283.1</v>
+        <v>30271.200000000001</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+        <v>357</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A260" s="3">
-        <v>30284.1</v>
+        <v>34825.1</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="176" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
-        <v>30290.1</v>
+        <v>30270.1</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A262" s="3">
-        <v>30296.2</v>
-      </c>
-      <c r="B262" s="2" t="s">
-        <v>374</v>
+        <v>359</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A262" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B262" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
-        <v>30297.1</v>
+        <v>30276.2</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="160" x14ac:dyDescent="0.2">
       <c r="A264" s="3">
-        <v>30970.2</v>
+        <v>34828.1</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="192" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
-        <v>34834.1</v>
+        <v>30275.200000000001</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266" s="3">
-        <v>28734.1</v>
-      </c>
-      <c r="B266" s="2" t="s">
-        <v>378</v>
+        <v>362</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A266" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B266" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
-        <v>28735.1</v>
+        <v>30291.200000000001</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>379</v>
+        <v>363</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="3">
-        <v>30978.2</v>
+        <v>34831.1</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>38</v>
+        <v>364</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
-        <v>34837.1</v>
+        <v>30281.1</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="3">
-        <v>30977.1</v>
+        <v>30282.1</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="3">
+        <v>30279.1</v>
+      </c>
       <c r="B271" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>38</v>
+        <v>367</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A272" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B272" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C272" s="5"/>
+      <c r="A272" s="3">
+        <v>30280.1</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B273" s="5" t="s">
-        <v>990</v>
-      </c>
-      <c r="C273" s="5"/>
+      <c r="A273" s="3">
+        <v>30286.1</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="3">
-        <v>29524.1</v>
+        <v>30287.1</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
-        <v>29827.1</v>
+        <v>30283.1</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>216</v>
+        <v>371</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="3">
-        <v>29501.200000000001</v>
+        <v>30284.1</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>134</v>
+        <v>372</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
-        <v>30192.2</v>
+        <v>30290.1</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="3">
-        <v>30193.200000000001</v>
+        <v>30296.2</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
-        <v>30194.2</v>
+        <v>30297.1</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A280" s="3">
-        <v>30200.2</v>
-      </c>
-      <c r="B280" s="2" t="s">
-        <v>388</v>
+      <c r="A280" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B280" s="12" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
-        <v>30195.200000000001</v>
+        <v>30970.2</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>389</v>
+        <v>376</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="3">
-        <v>33320.1</v>
+        <v>34834.1</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
-        <v>28939.200000000001</v>
+        <v>28734.1</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="3">
-        <v>30202.1</v>
+        <v>28735.1</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="C284" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B285" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" s="3">
+        <v>30978.2</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="C286" s="2" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A285" s="3">
-        <v>28879.1</v>
-      </c>
-      <c r="B285" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A286" s="3">
-        <v>28882.1</v>
-      </c>
-      <c r="B286" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
-        <v>30207.1</v>
+        <v>34837.1</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C287" s="2" t="s">
-        <v>38</v>
+        <v>381</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="3">
-        <v>28660.1</v>
+        <v>30977.1</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>396</v>
+        <v>382</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A289" s="3">
-        <v>28661.1</v>
-      </c>
       <c r="B289" s="2" t="s">
-        <v>397</v>
+        <v>383</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A290" s="3">
-        <v>31470.2</v>
-      </c>
-      <c r="B290" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="A290" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C290" s="5"/>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A291" s="3">
-        <v>31468.1</v>
-      </c>
-      <c r="B291" s="2" t="s">
-        <v>399</v>
-      </c>
+      <c r="A291" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B291" s="5" t="s">
+        <v>990</v>
+      </c>
+      <c r="C291" s="5"/>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="3">
-        <v>14447.1</v>
+        <v>29524.1</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="3">
-        <v>13980.1</v>
+        <v>29827.1</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>401</v>
+        <v>216</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="3">
-        <v>33314.1</v>
+        <v>29501.200000000001</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>402</v>
+        <v>134</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="3">
+        <v>30192.2</v>
+      </c>
       <c r="B295" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>38</v>
+        <v>385</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A296" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B296" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C296" s="5"/>
+      <c r="A296" s="3">
+        <v>30193.200000000001</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A297" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B297" s="5" t="s">
-        <v>991</v>
-      </c>
-      <c r="C297" s="5"/>
+      <c r="A297" s="3">
+        <v>30194.2</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="3">
-        <v>29524.1</v>
+        <v>30200.2</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="3">
-        <v>29501.200000000001</v>
+        <v>30195.200000000001</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>134</v>
+        <v>389</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="3">
-        <v>30214.1</v>
+        <v>33320.1</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="3">
-        <v>30217.1</v>
+        <v>28939.200000000001</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="3">
-        <v>30218.1</v>
+        <v>30202.1</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>407</v>
+        <v>392</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="3">
+        <v>28879.1</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A304" s="3">
+        <v>28882.1</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" s="3">
+        <v>30207.1</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C305" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" s="3">
+        <v>28660.1</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" s="3">
+        <v>28661.1</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" s="3">
+        <v>31470.2</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C308" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" s="3">
+        <v>31468.1</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" s="3">
+        <v>14447.1</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" s="3">
+        <v>13980.1</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" s="3">
+        <v>33314.1</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B313" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C313" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C314" s="5"/>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B315" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C315" s="5"/>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" s="3">
+        <v>29524.1</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" s="3">
+        <v>29501.200000000001</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" s="3">
+        <v>30214.1</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319" s="3">
+        <v>30217.1</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" s="3">
+        <v>30218.1</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="3">
         <v>30219.1</v>
       </c>
-      <c r="B303" s="2" t="s">
+      <c r="B321" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A304" s="3">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="3">
         <v>30221.1</v>
       </c>
-      <c r="B304" s="2" t="s">
+      <c r="B322" s="2" t="s">
         <v>409</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A305" s="3">
-        <v>30224.1</v>
-      </c>
-      <c r="B305" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A306" s="3">
-        <v>30223.1</v>
-      </c>
-      <c r="B306" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A307" s="3">
-        <v>31287.1</v>
-      </c>
-      <c r="B307" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A308" s="3">
-        <v>30226.1</v>
-      </c>
-      <c r="B308" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="3">
-        <v>30225.1</v>
-      </c>
-      <c r="B309" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A310" s="3">
-        <v>31288.1</v>
-      </c>
-      <c r="B310" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="3">
-        <v>30228.2</v>
-      </c>
-      <c r="B311" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="3">
-        <v>30227.200000000001</v>
-      </c>
-      <c r="B312" s="2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A313" s="3">
-        <v>28907.1</v>
-      </c>
-      <c r="B313" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A314" s="3">
-        <v>30230.1</v>
-      </c>
-      <c r="B314" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A315" s="3">
-        <v>30229.1</v>
-      </c>
-      <c r="B315" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A316" s="3">
-        <v>31290.1</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A317" s="3">
-        <v>30231.1</v>
-      </c>
-      <c r="B317" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A318" s="3">
-        <v>30239.1</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A319" s="3">
-        <v>30238.1</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A320" s="3">
-        <v>30237.1</v>
-      </c>
-      <c r="B320" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A321" s="3">
-        <v>30235.1</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A322" s="3">
-        <v>30234.1</v>
-      </c>
-      <c r="B322" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="3">
-        <v>30244.2</v>
+        <v>30224.1</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="3">
-        <v>30242.2</v>
+        <v>30223.1</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="3">
-        <v>30243.1</v>
+        <v>31287.1</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A326" s="3">
+        <v>30226.1</v>
+      </c>
       <c r="B326" s="2" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="3">
+        <v>30225.1</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A328" s="3">
+        <v>31288.1</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" s="3">
+        <v>30228.2</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="3">
+        <v>30227.200000000001</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A331" s="3">
+        <v>28907.1</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="3">
+        <v>30230.1</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="3">
+        <v>30229.1</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" s="3">
+        <v>31290.1</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="3">
+        <v>30231.1</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="3">
+        <v>30239.1</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A337" s="3">
+        <v>30238.1</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A338" s="3">
+        <v>30237.1</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A339" s="3">
+        <v>30235.1</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A340" s="3">
+        <v>30234.1</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A341" s="3">
+        <v>30244.2</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A342" s="3">
+        <v>30242.2</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A343" s="3">
+        <v>30243.1</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B344" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="3">
         <v>28583.1</v>
       </c>
-      <c r="B327" s="2" t="s">
+      <c r="B345" s="2" t="s">
         <v>432</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated cancer investigations template for missing elements - also further progress on cross references spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/rare diseases/GEL_openEHR_Cross_references.xlsx
+++ b/docs/rare diseases/GEL_openEHR_Cross_references.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Version Control" sheetId="24" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="1491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="1631">
   <si>
     <t>Full Name of Responsible Consultant (12774.4)</t>
   </si>
@@ -7862,6 +7862,1430 @@
   </si>
   <si>
     <t>RD sections complete</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0015]/value/id as Participant_identifier_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.participant_gel.v0]
+where a/name/value='GEL Cancer withdrawal'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/items[at0002]/value/value as Withdrawal_form
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains ADMIN_ENTRY b_a[openEHR-EHR-ADMIN_ENTRY.withdrawal_gel.v0]
+where a/name/value='GEL Cancer withdrawal'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/items[at0006]/value/value as Withdrawal_option
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains ADMIN_ENTRY b_a[openEHR-EHR-ADMIN_ENTRY.withdrawal_gel.v0]
+where a/name/value='GEL Cancer withdrawal'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/items[at0004]/value/value as Name_and_version_of_withdrawal_form
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains ADMIN_ENTRY b_a[openEHR-EHR-ADMIN_ENTRY.withdrawal_gel.v0]
+where a/name/value='GEL Cancer withdrawal'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/items[at0009]/value/value as Person_reporting_withdrawal
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains ADMIN_ENTRY b_a[openEHR-EHR-ADMIN_ENT</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0015]/value/id as Participant_identifier_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.participant_gel.v0]
+where a/name/value='GEL Cancer disease information update'</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0001]/value/value as Disease_type
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.disease_information_cancer_gel.v0]
+where a/name/value='GEL Cancer disease information update'</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0001]/value/id as Tumour_identifier_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.tumour_id_gel.v0]
+where a/name/value='GEL Cancer disease information update'</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0002]/value/value as Disease_subtype
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.disease_information_cancer_gel.v0]
+where a/name/value='GEL Cancer disease information update'</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0015]/value/id as Participant_identifier_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.participant_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/items[at0043]/value/value as Smoking
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains EVALUATION b_a[openEHR-EHR-EVALUATION.tobacco_smoking_summary.v1]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/items[at0029]/items[at0064]/items[at0023]/value/magnitude as Alcohol_consumption
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains EVALUATION b_a[openEHR-EHR-EVALUATION.alcohol_use_summary.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0004]/value/magnitude as Height
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.height.v1]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0002]/events[at0003]/data[at0001]/items[at0004]/value/magnitude as Weight
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.body_weight.v1]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0006]/value/value as Age_at_menarche
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0007]/value/value as Age_at_menopause
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0008]/value/value as Duration_of_OCP
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0009]/value/value as Duration_of_HRT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0010]/value/magnitude as Number_of_pregnancies
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0011]/value/magnitude as Number_of_births
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0029]/value/magnitude as Number_of_children_breastfed
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0030]/value/magnitude as Number_of_cycles_IVF
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0012]/value/value as Endometriosis
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0016]/value/value as Previous_tubal_ligation
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0020]/value/value as Use_of_IUD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0024]/value/value as Use_of_NSAIDs
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.ovarian_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0006]/value/value as Age_at_menarche
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0008]/value/value as Duration_of_OCP
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0009]/value/value as Duration_of_HRT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0010]/value/magnitude as Number_of_pregnancies
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0011]/value/magnitude as Number_of_births
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0029]/value/magnitude as Number_of_children_breastfed
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0030]/value/magnitude as Number_of_cycles_IVF
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0031]/value/value as Breast_density
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.breast_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0006]/value/value as Radiotherapy_in_childhood
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.glioma_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0006]/value/value as Age_at_menarche
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.endometrial_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0007]/value/value as Age_at_menopause
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.endometrial_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0008]/value/value as Duration_of_OCP
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.endometrial_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0009]/value/value as Duration_of_HRT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.endometrial_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0010]/value/magnitude as Number_of_pregnancies
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    OBSERVATION b_a[openEHR-EHR-OBSERVATION.endometrial_risk_gel.v0] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.female_cancer_risk_gel.v0])
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0037]/value/value as Tamoxifen_use_age
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.endometrial_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0006]/value/value as Dialysis_duration
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.renal_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0006]/value/value as Childhood_chronic_exposure
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.melanoma_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0007]/value/value as Sunbed_use_age
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.melanoma_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0008]/value/value as Skin_type
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.melanoma_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0006]/value/value as Cryptorchidism
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.testicular_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0010]/value/value as Cryptorchidism_correction_age
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.testicular_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0006]/value/value as Hepatitis_B_infection
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.hpb_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0011]/value/value as Hepatitis_C_infection
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.hpb_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>select
+    b_a/data[at0001]/events[at0002]/data[at0003]/items[at0016]/value/value as Cirrhosis
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains OBSERVATION b_a[openEHR-EHR-OBSERVATION.hpb_risk_gel.v0]
+where a/name/value='GEL Cancer risk factor assessment'</t>
+  </si>
+  <si>
+    <t>Cancer withdrawal, disease update, risk factors complete</t>
+  </si>
+  <si>
+    <t>select b_a/items[at0015]/value/id as Participant_identifier_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains CLUSTER b_a[openEHR-EHR-CLUSTER.participant_gel.v0]
+where a/name/value='GEL Cancer Investigations'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0005]/value/value as Imaging_Modality
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.imaging_exam.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001, 'Anatomical site']/value/value as Anatomical_site
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.anatomical_location.v1])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Anatomical_side
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.anatomical_side_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0002, 'Image file reference']/value/value as Image_file_reference
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.multimedia.v1])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0025]/items[at0027]/items[at0033, 'Imaging report reference']/value/id as Imaging_report_reference_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.imaging_exam.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0008]/value/value as Ultrasound_examination_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.imaging_exam.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0021]/value/value as Imaging_report_text
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.imaging_exam.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/id as Tumour_identifier_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tumour_id_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/items[at0002]/value/value/defining_code/code_string as Related_cancer_diagnosis_ICD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    EVALUATION b_b[openEHR-EHR-EVALUATION.problem_diagnosis.v1])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Related cancer diagnoses'</t>
+  </si>
+  <si>
+    <t>this assumes that ICD is the defining code terminology - if that is not the case, the value will have to be determined by mapping at runtime.</t>
+  </si>
+  <si>
+    <t>"select
+    b_a,
+    b_b/data[at0001]/items[at0002]/value/value/defining_code/code_string as Related_cancer_diagnosis_SNOMED_CT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    EVALUATION b_b[openEHR-EHR-EVALUATION.problem_diagnosis.v1])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Related cancer diagnoses'"</t>
+  </si>
+  <si>
+    <t>This assumes that SNOMED CT is the defining code terminology - if that is not the case, the value will have to be determined by mapping at runtime.</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0046]/items[at0001]/value/id as Local_sample_Id_id
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.specimen.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0015]/value/value as Sample_taken_date
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.specimen.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0046]/items[at0034]/value/value as Sample_receipt_date
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.specimen.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0004]/value/value/defining_code/code_string as Imaging_code_SNOMED_CT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.imaging_exam.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0004]/value/value/defining_code/code_string as Imaging_code_NICIP
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.imaging_exam.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>this assumes that SNOMED CT is the defining code terminology - if that is not the case, the value will have to be determined by mapping at runtime.</t>
+  </si>
+  <si>
+    <t>This assumes that NICIP is the defining code terminology - if that is not the case, the value will have to be determined by mapping at runtime.</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Mammogram_result
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.mammogram_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific imaging'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Lesion_location
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cns_result_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific imaging'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0050]/value/magnitude as Number_of_lesions
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cns_result_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific imaging'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0051]/value/value as Principal_diagnostic_imaging_type
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cns_result_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific imaging'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0055]/value/value as Feature_of_largest_lesion
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cns_result_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific imaging'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0066]/value/magnitude as Lesion_size
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cns_result_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific imaging'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0098]/value/value/defining_code/code_string as Primary_diagnosis_ICD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.laboratory_test.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0098]/value/value/defining_code/code_string as Primary_diagnosis_SNOMED_CT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.laboratory_test.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/data[at0001]/events[at0002]/data[at0003]/items[at0077]/value/value as Pathology_investigation_type
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.laboratory_test.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0005]/value/value as Excision_margin
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0005]/value/value as Grade_of_differentiation
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tnm_stage_pathological.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value as Pathology_report
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.multimedia.v1])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/items[at0003]/value/magnitude as Number_of_nodes_examined
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/items[at0002]/value/magnitude as Number_of_nodes_positive
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value as Pathology_image_file_reference
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.multimedia.v1])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0020]/value/value as Tumour_type
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0019]/value/value as Pre_operative_therapy
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/data[at0001]/origin/value as Investigation_result_date
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.laboratory_test.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/protocol[at0004]/items[at0094]/items[at0063]/value as Receiver_order_identifier
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    OBSERVATION b_b[openEHR-EHR-OBSERVATION.laboratory_test.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0028]/value/value as Cancer_vascular_or_lymphatic_invasion
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0018]/value/magnitude as Tumour_size
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0037]/value/value as Pre_invasive_elements
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gel_histopath_summary.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value as Tumour_identifier
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tumour_id_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value/defining_code/code_string as Morphology_ICD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value/defining_code/code_string as Morphology_SNOMED_CT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value/defining_code/code_string as Morphology_SNOMED_RT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value/defining_code/code_string as Morphology_SNOMED
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>This assumes that SNOMED RT is the defining code terminology - if that is not the case, the value will have to be determined by mapping at runtime.</t>
+  </si>
+  <si>
+    <t>This assumes that SNOMED (earlier versions than RT and CT) is the defining code terminology - if that is not the case, the value will have to be determined by mapping at runtime.</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0002]/value/value/defining_code/code_string as Topography_ICD
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0002]/value/value/defining_code/code_string as Topography_SNOMED_CT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0002]/value/value/defining_code/code_string as Topography_SNOMED_RT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0002]/value/value/defining_code/code_string as Topography_SNOMED
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.cancer_diagnosis_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0016]/value/value as TNM_edition
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tnm_stage_pathological.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as Primary_tumour_pT
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tnm_stage_pathological.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0002]/value/value as Regional_lymph_node_pN
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tnm_stage_pathological.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0003]/value/value as Distant_metastasis_pM
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tnm_stage_pathological.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='General'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as MLH1_IHC_1
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.colorectal_tm_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0006]/value/value as MLH1_IHC_2
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.colorectal_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0011]/value/value as MSH6_IHC
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.colorectal_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0016]/value/value as PMS2_IHC
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.colorectal_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as WT1_IHC
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ovarian_tm_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as Epidermal_growth_factor_receptor_mutational_status
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.lung_tm_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Molecular_subgroup
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.childhood_tm_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0007]/value/value as TP53
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.childhood_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0011]/value/value as MYC
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.childhood_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0015]/value/value as MYCN
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.childhood_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0019]/value/value as ALK
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.childhood_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0023]/value/value as Chromosomal_abnormality
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.childhood_tm_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific tumour markers'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0166]/value/value as Primary_Gleason_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gleason_score.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0182]/value/value as Secondary_Gleason_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.gleason_score.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Fuhrman_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.fuhrman.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as FIGO_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.figo_grade.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Invasive_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.invasive_grade_breast.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as DCIS_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.dcis_grade.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as Serum_tumour_markers
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.serum_tm.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as WHO_CNS_tumour_markers
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.who_cns_tm.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as WHO_glioma_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.glioma_who2007.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Sarcomatoid_change
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.sarcomatoid_change.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as Histopathological_tumour_grade
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.tumour_grade_sarcoma.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0019]/value/magnitude as Leibovich_score
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.leibovich.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Tumour_grade_urology
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.urology_grade.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Tumour_grade_ovarian_serous
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.ovarian_serous_grade.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific grading'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0001]/value/value as Detrusor_muscle_presence_indicator
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.bladder_cancer_pathology_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific pathology'</t>
+  </si>
+  <si>
+    <t>select b_a, b_b/items[at0001]/value/value as Core_biopsy_breast
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.breast_cancer_pathology_gel.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific pathology'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0009]/value/value as Core_biopsy_node
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.breast_cancer_pathology_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific pathology'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0015]/value/value as Cytology_node
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.breast_cancer_pathology_gel.v0])
+where
+    a/name/value='GEL Cancer Investigations' and
+    b_a/name/value='Cancer-specific pathology'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0013]/value/magnitude as PR_ALLRED_score
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.pr_allred_score.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific pathology'</t>
+  </si>
+  <si>
+    <t>select
+    b_a,
+    b_b/items[at0013]/value/magnitude as ER_ALLRED_score
+from EHR e
+contains COMPOSITION a[openEHR-EHR-COMPOSITION.report.v1]
+contains (
+    SECTION b_a[openEHR-EHR-SECTION.adhoc.v1] and
+    CLUSTER b_b[openEHR-EHR-CLUSTER.er_allred_score.v0])
+where a/name/value='GEL Cancer Investigations'
+and b_a/name/value='Cancer-specific pathology'</t>
   </si>
 </sst>
 </file>
@@ -8375,8 +9799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8432,8 +9856,15 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>43013</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1541</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
@@ -8480,8 +9911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8667,7 +10098,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8691,51 +10122,63 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>531</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>1491</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>554</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>549</v>
       </c>
+      <c r="C3" s="6" t="s">
+        <v>1492</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>555</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>550</v>
       </c>
+      <c r="C4" s="6" t="s">
+        <v>1493</v>
+      </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>556</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>551</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="5" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>557</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>1495</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
@@ -8795,7 +10238,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8819,41 +10262,51 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>531</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>1496</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>561</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>1497</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>562</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>559</v>
       </c>
+      <c r="C4" s="6" t="s">
+        <v>1499</v>
+      </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>563</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>560</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1498</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -8929,17 +10382,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="43" style="6" customWidth="1"/>
-    <col min="3" max="3" width="99.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="21.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43" style="2" customWidth="1"/>
+    <col min="3" max="3" width="99.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -8954,50 +10407,63 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>531</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>1500</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>1501</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>569</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>565</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>1502</v>
+      </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>566</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>1503</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>571</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>567</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1504</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -9006,350 +10472,480 @@
       <c r="B7" s="5" t="s">
         <v>1135</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>1136</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="112" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>1383</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>1137</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>1138</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="5" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>1385</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>1139</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>1386</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>1140</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="5" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>1387</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>1141</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="5" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>1388</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="5" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>1389</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="5" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>1390</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>1144</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" s="5" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>1391</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>1145</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="C17" s="5" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>14482</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>1146</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="C18" s="2" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>29104</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>1147</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
+      <c r="C19" s="2" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>29105</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>1148</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>1512</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>1149</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
+      <c r="C21" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>14473</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>1150</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
+      <c r="C22" s="2" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>14474</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>1151</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
+      <c r="C23" s="2" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>14475</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>1139</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
+      <c r="C24" s="2" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>14476</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>1140</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
+      <c r="C25" s="2" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>14477</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
+      <c r="C26" s="2" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>14478</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>1152</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
+      <c r="C27" s="2" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>29104</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>1147</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
+      <c r="C28" s="2" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>29105</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>1148</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
+      <c r="C29" s="2" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>29108</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>1153</v>
       </c>
+      <c r="C30" s="2" t="s">
+        <v>1524</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>1154</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
+      <c r="C31" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <v>38863</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>1155</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
+      <c r="C32" s="2" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
         <v>1156</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
+      <c r="C33" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
         <v>14473</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>1150</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
+      <c r="C34" s="2" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>14474</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>1151</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
+      <c r="C35" s="2" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>14475</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>1139</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
+      <c r="C36" s="2" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>14476</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>1140</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
+      <c r="C37" s="2" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="144" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>14477</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>1141</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
+      <c r="C38" s="2" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>39005</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>1157</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+      <c r="C39" s="2" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
+      <c r="C40" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>39011</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="2" t="s">
         <v>1159</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="6" t="s">
+      <c r="C41" s="2" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
         <v>1160</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
+      <c r="C42" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
         <v>39012</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="2" t="s">
         <v>1161</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
+      <c r="C43" s="2" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
         <v>39014</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="2" t="s">
         <v>1162</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
+      <c r="C44" s="2" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
         <v>39016</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="2" t="s">
         <v>1163</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="6" t="s">
+      <c r="C45" s="2" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
         <v>1164</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
+      <c r="C46" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
         <v>39019</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="2" t="s">
         <v>1165</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
+      <c r="C47" s="2" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
         <v>39097</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>1166</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="6" t="s">
+      <c r="C48" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
         <v>1167</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
+      <c r="C49" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
         <v>39025</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="2" t="s">
         <v>1168</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
+      <c r="C50" s="2" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
         <v>39028</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="2" t="s">
         <v>1169</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
+      <c r="C51" s="2" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
         <v>39030</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="2" t="s">
         <v>1170</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>1540</v>
       </c>
     </row>
   </sheetData>
@@ -9361,17 +10957,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="43" style="6" customWidth="1"/>
-    <col min="3" max="3" width="99.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="21.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="43" style="2" customWidth="1"/>
+    <col min="3" max="3" width="99.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -9386,14 +10982,16 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>531</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>1542</v>
+      </c>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9401,74 +10999,100 @@
       <c r="B3" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>777</v>
+      </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>573</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>1543</v>
+      </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>574</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>1544</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>575</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>1545</v>
+      </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>723</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>724</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>725</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>726</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="128" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>563</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>560</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1550</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -9477,22 +11101,36 @@
       <c r="B12" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="5" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>727</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>728</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>582</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1554</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -9500,1244 +11138,1552 @@
       <c r="B15" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>777</v>
+      </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="160" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>729</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>584</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>1555</v>
+      </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>730</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>585</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>1556</v>
+      </c>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+    <row r="18" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>12761</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>586</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>1557</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
+      <c r="C19" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>12752</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
+      <c r="C20" s="2" t="s">
+        <v>1558</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>33449</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>589</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1561</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>1171</v>
       </c>
+      <c r="C22" s="2" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
+      <c r="C23" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>38883</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>1173</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>1562</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>1174</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="C25" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>1175</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="C26" s="2" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>1256</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>1176</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="C27" s="2" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>1257</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>1177</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="C28" s="2" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>1258</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>1178</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="C29" s="2" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>1259</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>1179</v>
       </c>
+      <c r="C30" s="2" t="s">
+        <v>1567</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
+      <c r="C31" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <v>38876</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="C32" s="2" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
+      <c r="C33" s="2" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
         <v>14903</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
+      <c r="C34" s="2" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>13904</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
+      <c r="C35" s="2" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>14905</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
+      <c r="C36" s="2" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>14907</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
+      <c r="C37" s="2" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>14908</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
+      <c r="C38" s="2" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>38882</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
+      <c r="C39" s="2" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
         <v>14912</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="2" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
+      <c r="C40" s="2" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>14721</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="2" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
+      <c r="C41" s="2" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
         <v>35534</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="2" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
+      <c r="C42" s="2" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
         <v>40107</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="2" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
+      <c r="C43" s="2" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
         <v>39088</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="2" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
+      <c r="C44" s="2" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
         <v>38881</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="2" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
+      <c r="C45" s="2" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
         <v>29075</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="2" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
+      <c r="C46" s="2" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
         <v>14872</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="2" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
+      <c r="C47" s="2" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
         <v>42230</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="6" t="s">
+      <c r="C48" s="2" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
+      <c r="C49" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
         <v>14871</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="2" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
+      <c r="C50" s="2" t="s">
+        <v>1585</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
         <v>31244</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="2" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
+      <c r="C51" s="2" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
         <v>31243</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="2" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
+      <c r="C52" s="2" t="s">
+        <v>1587</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
         <v>42048</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="2" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
+      <c r="C53" s="2" t="s">
+        <v>1588</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
         <v>42049</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="2" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="6" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
+      <c r="C55" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
         <v>31228</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="2" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="7">
+      <c r="C56" s="2" t="s">
+        <v>1591</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
         <v>14876</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="2" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
+      <c r="C57" s="2" t="s">
+        <v>1592</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
         <v>31227</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="2" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="7">
+      <c r="C58" s="2" t="s">
+        <v>1593</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
         <v>42052</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="2" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="7">
+      <c r="C59" s="2" t="s">
+        <v>1594</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
         <v>42049</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="2" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B61" s="6" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="7">
+      <c r="C61" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
         <v>14909</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="2" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" s="7">
+      <c r="C62" s="2" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
         <v>14910</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="2" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" s="7">
+      <c r="C63" s="2" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="176" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
         <v>14911</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="2" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="7">
+      <c r="C64" s="2" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
         <v>29098</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="2" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="6" t="s">
+      <c r="C65" s="2" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
         <v>1180</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B67" s="6" t="s">
+      <c r="C66" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="s">
         <v>1181</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+      <c r="C67" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>1260</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="2" t="s">
         <v>1182</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
+      <c r="C68" s="2" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>1261</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="2" t="s">
         <v>1183</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="7" t="s">
+      <c r="C69" s="2" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>1262</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="2" t="s">
         <v>1184</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
+      <c r="C70" s="2" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>1263</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="2" t="s">
         <v>1185</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="6" t="s">
+      <c r="C71" s="2" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B72" s="2" t="s">
         <v>1186</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
+      <c r="C72" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>1264</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="2" t="s">
         <v>1187</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="6" t="s">
+      <c r="C73" s="2" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B74" s="2" t="s">
         <v>1188</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="C74" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>1265</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="2" t="s">
         <v>1189</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="6" t="s">
+      <c r="C75" s="2" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B76" s="2" t="s">
         <v>1190</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+      <c r="C76" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>1266</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="2" t="s">
         <v>1191</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
+      <c r="C77" s="2" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>1267</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="2" t="s">
         <v>1192</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
+      <c r="C78" s="2" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>1268</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="2" t="s">
         <v>1193</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+      <c r="C79" s="2" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
         <v>1269</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="2" t="s">
         <v>1194</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
+      <c r="C80" s="2" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>1270</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B81" s="2" t="s">
         <v>1195</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A82" s="7" t="s">
+      <c r="C81" s="2" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>1271</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="2" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="6" t="s">
+      <c r="C82" s="2" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B83" s="2" t="s">
         <v>1197</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="6" t="s">
+      <c r="C83" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B84" s="2" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" s="7" t="s">
+      <c r="C84" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>1272</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="2" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+      <c r="C85" s="2" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
         <v>1273</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="2" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" s="7" t="s">
+      <c r="C86" s="2" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>1274</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="2" t="s">
         <v>1198</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
+      <c r="C87" s="2" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>1275</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="2" t="s">
         <v>1199</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="7" t="s">
+      <c r="C88" s="2" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
         <v>1276</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="2" t="s">
         <v>1200</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
+      <c r="C89" s="2" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>1277</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="2" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" s="7" t="s">
+      <c r="C90" s="2" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>1278</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="2" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
+      <c r="C91" s="2" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>1279</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="2" t="s">
         <v>1203</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" s="7" t="s">
+      <c r="C92" s="2" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>1280</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="2" t="s">
         <v>1204</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
+      <c r="C93" s="2" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>1281</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B94" s="2" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" s="7" t="s">
+      <c r="C94" s="2" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>1282</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="2" t="s">
         <v>1206</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
+      <c r="C95" s="2" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>1283</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B96" s="2" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
+      <c r="C96" s="2" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
         <v>1284</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B97" s="2" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="7" t="s">
+      <c r="C97" s="2" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
         <v>1285</v>
       </c>
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="2" t="s">
         <v>1209</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="6" t="s">
+      <c r="C98" s="2" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B99" s="2" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="6" t="s">
+      <c r="C99" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B100" s="2" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="C100" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>1286</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="2" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="6" t="s">
+      <c r="C101" s="2" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B102" s="2" t="s">
         <v>1213</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
+      <c r="C102" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="128" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>1287</v>
       </c>
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="2" t="s">
         <v>1214</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
+      <c r="C103" s="2" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>1288</v>
       </c>
-      <c r="B104" s="6" t="s">
+      <c r="B104" s="2" t="s">
         <v>1215</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
+      <c r="C104" s="2" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="176" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>1289</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="2" t="s">
         <v>1216</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="7" t="s">
+      <c r="C105" s="2" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
         <v>1290</v>
       </c>
-      <c r="B106" s="6" t="s">
+      <c r="B106" s="2" t="s">
         <v>1217</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
+      <c r="C106" s="2" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="160" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
         <v>1291</v>
       </c>
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="2" t="s">
         <v>1218</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
+      <c r="C107" s="2" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>1292</v>
       </c>
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="2" t="s">
         <v>1219</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>1293</v>
       </c>
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="2" t="s">
         <v>1220</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="7" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>1294</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B110" s="2" t="s">
         <v>1221</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B111" s="6" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B111" s="2" t="s">
         <v>1222</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="7" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>1295</v>
       </c>
-      <c r="B112" s="6" t="s">
+      <c r="B112" s="2" t="s">
         <v>1223</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B113" s="6" t="s">
+      <c r="B113" s="2" t="s">
         <v>1224</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+      <c r="A114" s="3" t="s">
         <v>1296</v>
       </c>
-      <c r="B114" s="6" t="s">
+      <c r="B114" s="2" t="s">
         <v>1225</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="3" t="s">
         <v>1297</v>
       </c>
-      <c r="B115" s="6" t="s">
+      <c r="B115" s="2" t="s">
         <v>1226</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="3" t="s">
         <v>1298</v>
       </c>
-      <c r="B116" s="6" t="s">
+      <c r="B116" s="2" t="s">
         <v>1227</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
+      <c r="A117" s="3" t="s">
         <v>1299</v>
       </c>
-      <c r="B117" s="6" t="s">
+      <c r="B117" s="2" t="s">
         <v>1228</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="3" t="s">
         <v>1300</v>
       </c>
-      <c r="B118" s="6" t="s">
+      <c r="B118" s="2" t="s">
         <v>1229</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B119" s="6" t="s">
+      <c r="B119" s="2" t="s">
         <v>1230</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
+      <c r="A120" s="3" t="s">
         <v>1301</v>
       </c>
-      <c r="B120" s="6" t="s">
+      <c r="B120" s="2" t="s">
         <v>1231</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
+      <c r="A121" s="3" t="s">
         <v>1302</v>
       </c>
-      <c r="B121" s="6" t="s">
+      <c r="B121" s="2" t="s">
         <v>1232</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
+      <c r="A122" s="3" t="s">
         <v>1303</v>
       </c>
-      <c r="B122" s="6" t="s">
+      <c r="B122" s="2" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
+      <c r="A123" s="3" t="s">
         <v>1304</v>
       </c>
-      <c r="B123" s="6" t="s">
+      <c r="B123" s="2" t="s">
         <v>1234</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
+      <c r="A124" s="3" t="s">
         <v>1305</v>
       </c>
-      <c r="B124" s="6" t="s">
+      <c r="B124" s="2" t="s">
         <v>1235</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
+      <c r="A125" s="3" t="s">
         <v>1306</v>
       </c>
-      <c r="B125" s="6" t="s">
+      <c r="B125" s="2" t="s">
         <v>1236</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="7" t="s">
+      <c r="A126" s="3" t="s">
         <v>1307</v>
       </c>
-      <c r="B126" s="6" t="s">
+      <c r="B126" s="2" t="s">
         <v>1237</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="3" t="s">
         <v>1308</v>
       </c>
-      <c r="B127" s="6" t="s">
+      <c r="B127" s="2" t="s">
         <v>1238</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="7" t="s">
+      <c r="A128" s="3" t="s">
         <v>1309</v>
       </c>
-      <c r="B128" s="6" t="s">
+      <c r="B128" s="2" t="s">
         <v>1239</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B129" s="6" t="s">
+      <c r="B129" s="2" t="s">
         <v>1240</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="7" t="s">
+      <c r="A130" s="3" t="s">
         <v>1310</v>
       </c>
-      <c r="B130" s="6" t="s">
+      <c r="B130" s="2" t="s">
         <v>1241</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="7" t="s">
+      <c r="A131" s="3" t="s">
         <v>1311</v>
       </c>
-      <c r="B131" s="6" t="s">
+      <c r="B131" s="2" t="s">
         <v>1242</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="7" t="s">
+      <c r="A132" s="3" t="s">
         <v>1312</v>
       </c>
-      <c r="B132" s="6" t="s">
+      <c r="B132" s="2" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
+      <c r="A133" s="3" t="s">
         <v>1313</v>
       </c>
-      <c r="B133" s="6" t="s">
+      <c r="B133" s="2" t="s">
         <v>1244</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B134" s="6" t="s">
+      <c r="B134" s="2" t="s">
         <v>1245</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
+      <c r="A135" s="3" t="s">
         <v>1314</v>
       </c>
-      <c r="B135" s="6" t="s">
+      <c r="B135" s="2" t="s">
         <v>1246</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A136" s="7" t="s">
+      <c r="A136" s="3" t="s">
         <v>1315</v>
       </c>
-      <c r="B136" s="6" t="s">
+      <c r="B136" s="2" t="s">
         <v>1247</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A137" s="7" t="s">
+      <c r="A137" s="3" t="s">
         <v>1316</v>
       </c>
-      <c r="B137" s="6" t="s">
+      <c r="B137" s="2" t="s">
         <v>1248</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B138" s="6" t="s">
+      <c r="B138" s="2" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A139" s="7" t="s">
+      <c r="A139" s="3" t="s">
         <v>1317</v>
       </c>
-      <c r="B139" s="6" t="s">
+      <c r="B139" s="2" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A140" s="7" t="s">
+      <c r="A140" s="3" t="s">
         <v>1318</v>
       </c>
-      <c r="B140" s="6" t="s">
+      <c r="B140" s="2" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A141" s="7" t="s">
+      <c r="A141" s="3" t="s">
         <v>1319</v>
       </c>
-      <c r="B141" s="6" t="s">
+      <c r="B141" s="2" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A142" s="7" t="s">
+      <c r="A142" s="3" t="s">
         <v>1320</v>
       </c>
-      <c r="B142" s="6" t="s">
+      <c r="B142" s="2" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A143" s="7" t="s">
+      <c r="A143" s="3" t="s">
         <v>1321</v>
       </c>
-      <c r="B143" s="6" t="s">
+      <c r="B143" s="2" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B144" s="6" t="s">
+      <c r="B144" s="2" t="s">
         <v>1250</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A145" s="7" t="s">
+      <c r="A145" s="3" t="s">
         <v>1322</v>
       </c>
-      <c r="B145" s="6" t="s">
+      <c r="B145" s="2" t="s">
         <v>1251</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B146" s="6" t="s">
+      <c r="B146" s="2" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A147" s="7">
+      <c r="A147" s="3">
         <v>42230</v>
       </c>
-      <c r="B147" s="6" t="s">
+      <c r="B147" s="2" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A148" s="7">
+      <c r="A148" s="3">
         <v>4563</v>
       </c>
-      <c r="B148" s="6" t="s">
+      <c r="B148" s="2" t="s">
         <v>631</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A149" s="7">
+      <c r="A149" s="3">
         <v>6101</v>
       </c>
-      <c r="B149" s="6" t="s">
+      <c r="B149" s="2" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A150" s="7">
+      <c r="A150" s="3">
         <v>12764</v>
       </c>
-      <c r="B150" s="6" t="s">
+      <c r="B150" s="2" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A151" s="7">
+      <c r="A151" s="3">
         <v>12765</v>
       </c>
-      <c r="B151" s="6" t="s">
+      <c r="B151" s="2" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="7">
+      <c r="A152" s="3">
         <v>12744</v>
       </c>
-      <c r="B152" s="6" t="s">
+      <c r="B152" s="2" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A153" s="7">
+      <c r="A153" s="3">
         <v>14900</v>
       </c>
-      <c r="B153" s="6" t="s">
+      <c r="B153" s="2" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A154" s="7">
+      <c r="A154" s="3">
         <v>34224</v>
       </c>
-      <c r="B154" s="6" t="s">
+      <c r="B154" s="2" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" s="7">
+      <c r="A155" s="3">
         <v>34225</v>
       </c>
-      <c r="B155" s="6" t="s">
+      <c r="B155" s="2" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B156" s="6" t="s">
+      <c r="B156" s="2" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" s="7">
+      <c r="A157" s="3">
         <v>12766</v>
       </c>
-      <c r="B157" s="6" t="s">
+      <c r="B157" s="2" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" s="7">
+      <c r="A158" s="3">
         <v>12767</v>
       </c>
-      <c r="B158" s="6" t="s">
+      <c r="B158" s="2" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" s="7">
+      <c r="A159" s="3">
         <v>5182</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="B159" s="2" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" s="7">
+      <c r="A160" s="3">
         <v>42230</v>
       </c>
-      <c r="B160" s="6" t="s">
+      <c r="B160" s="2" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" s="7" t="s">
+      <c r="A161" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="B161" s="6" t="s">
+      <c r="B161" s="2" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" s="7">
+      <c r="A162" s="3">
         <v>14629</v>
       </c>
-      <c r="B162" s="6" t="s">
+      <c r="B162" s="2" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="7">
+      <c r="A163" s="3">
         <v>38916</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B163" s="2" t="s">
         <v>645</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" s="7">
+      <c r="A164" s="3">
         <v>42230</v>
       </c>
-      <c r="B164" s="6" t="s">
+      <c r="B164" s="2" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B165" s="6" t="s">
+      <c r="B165" s="2" t="s">
         <v>1252</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" s="7" t="s">
+      <c r="A166" s="3" t="s">
         <v>1254</v>
       </c>
-      <c r="B166" s="6" t="s">
+      <c r="B166" s="2" t="s">
         <v>1253</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" s="7" t="s">
+      <c r="A167" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="B167" s="6" t="s">
+      <c r="B167" s="2" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" s="7">
+      <c r="A168" s="3">
         <v>33106</v>
       </c>
-      <c r="B168" s="6" t="s">
+      <c r="B168" s="2" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" s="7">
+      <c r="A169" s="3">
         <v>33096</v>
       </c>
-      <c r="B169" s="6" t="s">
+      <c r="B169" s="2" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" s="7">
+      <c r="A170" s="3">
         <v>33454</v>
       </c>
-      <c r="B170" s="6" t="s">
+      <c r="B170" s="2" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" s="7">
+      <c r="A171" s="3">
         <v>42230</v>
       </c>
-      <c r="B171" s="6" t="s">
+      <c r="B171" s="2" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" s="7">
+      <c r="A172" s="3">
         <v>33104</v>
       </c>
-      <c r="B172" s="6" t="s">
+      <c r="B172" s="2" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" s="7">
+      <c r="A173" s="3">
         <v>33097</v>
       </c>
-      <c r="B173" s="6" t="s">
+      <c r="B173" s="2" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" s="7">
+      <c r="A174" s="3">
         <v>33098</v>
       </c>
-      <c r="B174" s="6" t="s">
+      <c r="B174" s="2" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="7">
+      <c r="A175" s="3">
         <v>33100</v>
       </c>
-      <c r="B175" s="6" t="s">
+      <c r="B175" s="2" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="7">
+      <c r="A176" s="3">
         <v>33455</v>
       </c>
-      <c r="B176" s="6" t="s">
+      <c r="B176" s="2" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" s="7">
+      <c r="A177" s="3">
         <v>33101</v>
       </c>
-      <c r="B177" s="6" t="s">
+      <c r="B177" s="2" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A178" s="7">
+      <c r="A178" s="3">
         <v>33102</v>
       </c>
-      <c r="B178" s="6" t="s">
+      <c r="B178" s="2" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A179" s="7">
+      <c r="A179" s="3">
         <v>33456</v>
       </c>
-      <c r="B179" s="6" t="s">
+      <c r="B179" s="2" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A180" s="7">
+      <c r="A180" s="3">
         <v>33099</v>
       </c>
-      <c r="B180" s="6" t="s">
+      <c r="B180" s="2" t="s">
         <v>657</v>
       </c>
     </row>
@@ -11976,7 +13922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -13032,7 +14978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -17657,8 +19603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="B11" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>